<commit_message>
source import & other imports updates
</commit_message>
<xml_diff>
--- a/assets/templates/import-incomes-template.xlsx
+++ b/assets/templates/import-incomes-template.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t xml:space="preserve">Waterfall ID</t>
   </si>
@@ -48,6 +48,9 @@
       </rPr>
       <t xml:space="preserve">// Root contract ID</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Source ID</t>
   </si>
   <si>
     <r>
@@ -389,18 +392,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A10:AL40"/>
+  <dimension ref="A10:AM40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J14" activeCellId="0" sqref="J14"/>
+      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.97"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="20.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.86"/>
   </cols>
   <sheetData>
     <row r="10" customFormat="false" ht="60" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -413,16 +416,16 @@
       <c r="C10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="G10" s="2" t="s">
         <v>6</v>
       </c>
       <c r="H10" s="1" t="s">
@@ -431,18 +434,20 @@
       <c r="I10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J10" s="3"/>
+      <c r="J10" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="K10" s="3"/>
-      <c r="L10" s="4"/>
+      <c r="L10" s="3"/>
       <c r="M10" s="4"/>
-      <c r="N10" s="5"/>
+      <c r="N10" s="4"/>
       <c r="O10" s="5"/>
       <c r="P10" s="5"/>
-      <c r="Q10" s="6"/>
-      <c r="R10" s="7"/>
+      <c r="Q10" s="5"/>
+      <c r="R10" s="6"/>
       <c r="S10" s="7"/>
-      <c r="T10" s="8"/>
-      <c r="U10" s="9"/>
+      <c r="T10" s="7"/>
+      <c r="U10" s="8"/>
       <c r="V10" s="9"/>
       <c r="W10" s="9"/>
       <c r="X10" s="9"/>
@@ -460,6 +465,7 @@
       <c r="AJ10" s="9"/>
       <c r="AK10" s="9"/>
       <c r="AL10" s="9"/>
+      <c r="AM10" s="9"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="10"/>
@@ -471,6 +477,7 @@
       <c r="G11" s="10"/>
       <c r="H11" s="10"/>
       <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="10"/>
@@ -482,6 +489,7 @@
       <c r="G12" s="10"/>
       <c r="H12" s="10"/>
       <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="10"/>
@@ -493,6 +501,7 @@
       <c r="G13" s="10"/>
       <c r="H13" s="10"/>
       <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="10"/>
@@ -504,6 +513,7 @@
       <c r="G14" s="10"/>
       <c r="H14" s="10"/>
       <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="10"/>
@@ -515,6 +525,7 @@
       <c r="G15" s="10"/>
       <c r="H15" s="10"/>
       <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="10"/>
@@ -526,6 +537,7 @@
       <c r="G16" s="10"/>
       <c r="H16" s="10"/>
       <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="10"/>
@@ -537,6 +549,7 @@
       <c r="G17" s="10"/>
       <c r="H17" s="10"/>
       <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="10"/>
@@ -548,6 +561,7 @@
       <c r="G18" s="10"/>
       <c r="H18" s="10"/>
       <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="10"/>
@@ -559,6 +573,7 @@
       <c r="G19" s="10"/>
       <c r="H19" s="10"/>
       <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="10"/>
@@ -570,6 +585,7 @@
       <c r="G20" s="10"/>
       <c r="H20" s="10"/>
       <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="10"/>
@@ -581,6 +597,7 @@
       <c r="G21" s="10"/>
       <c r="H21" s="10"/>
       <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="10"/>
@@ -592,6 +609,7 @@
       <c r="G22" s="10"/>
       <c r="H22" s="10"/>
       <c r="I22" s="10"/>
+      <c r="J22" s="10"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="10"/>
@@ -603,6 +621,7 @@
       <c r="G23" s="10"/>
       <c r="H23" s="10"/>
       <c r="I23" s="10"/>
+      <c r="J23" s="10"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="10"/>
@@ -614,6 +633,7 @@
       <c r="G24" s="10"/>
       <c r="H24" s="10"/>
       <c r="I24" s="10"/>
+      <c r="J24" s="10"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="10"/>
@@ -625,6 +645,7 @@
       <c r="G25" s="10"/>
       <c r="H25" s="10"/>
       <c r="I25" s="10"/>
+      <c r="J25" s="10"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="10"/>
@@ -636,6 +657,7 @@
       <c r="G26" s="10"/>
       <c r="H26" s="10"/>
       <c r="I26" s="10"/>
+      <c r="J26" s="10"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="10"/>
@@ -647,6 +669,7 @@
       <c r="G27" s="10"/>
       <c r="H27" s="10"/>
       <c r="I27" s="10"/>
+      <c r="J27" s="10"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="10"/>
@@ -658,6 +681,7 @@
       <c r="G28" s="10"/>
       <c r="H28" s="10"/>
       <c r="I28" s="10"/>
+      <c r="J28" s="10"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="10"/>
@@ -669,6 +693,7 @@
       <c r="G29" s="10"/>
       <c r="H29" s="10"/>
       <c r="I29" s="10"/>
+      <c r="J29" s="10"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="10"/>
@@ -680,6 +705,7 @@
       <c r="G30" s="10"/>
       <c r="H30" s="10"/>
       <c r="I30" s="10"/>
+      <c r="J30" s="10"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="10"/>
@@ -691,6 +717,7 @@
       <c r="G31" s="10"/>
       <c r="H31" s="10"/>
       <c r="I31" s="10"/>
+      <c r="J31" s="10"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="10"/>
@@ -702,6 +729,7 @@
       <c r="G32" s="10"/>
       <c r="H32" s="10"/>
       <c r="I32" s="10"/>
+      <c r="J32" s="10"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="10"/>
@@ -713,6 +741,7 @@
       <c r="G33" s="10"/>
       <c r="H33" s="10"/>
       <c r="I33" s="10"/>
+      <c r="J33" s="10"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="10"/>
@@ -724,6 +753,7 @@
       <c r="G34" s="10"/>
       <c r="H34" s="10"/>
       <c r="I34" s="10"/>
+      <c r="J34" s="10"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="10"/>
@@ -735,6 +765,7 @@
       <c r="G35" s="10"/>
       <c r="H35" s="10"/>
       <c r="I35" s="10"/>
+      <c r="J35" s="10"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="10"/>
@@ -746,6 +777,7 @@
       <c r="G36" s="10"/>
       <c r="H36" s="10"/>
       <c r="I36" s="10"/>
+      <c r="J36" s="10"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="10"/>
@@ -757,6 +789,7 @@
       <c r="G37" s="10"/>
       <c r="H37" s="10"/>
       <c r="I37" s="10"/>
+      <c r="J37" s="10"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="10"/>
@@ -768,6 +801,7 @@
       <c r="G38" s="10"/>
       <c r="H38" s="10"/>
       <c r="I38" s="10"/>
+      <c r="J38" s="10"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="10"/>
@@ -779,6 +813,7 @@
       <c r="G39" s="10"/>
       <c r="H39" s="10"/>
       <c r="I39" s="10"/>
+      <c r="J39" s="10"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="10"/>
@@ -790,6 +825,7 @@
       <c r="G40" s="10"/>
       <c r="H40" s="10"/>
       <c r="I40" s="10"/>
+      <c r="J40" s="10"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Feat 9420 actions import (#9438)
* added id on waterfall sources

* source import & other imports updates

* debug

* debug & cleaning & improvements

---------

Co-authored-by: bruce <delorme.bruce.michel@gmail.com>
</commit_message>
<xml_diff>
--- a/assets/templates/import-incomes-template.xlsx
+++ b/assets/templates/import-incomes-template.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t xml:space="preserve">Waterfall ID</t>
   </si>
@@ -48,6 +48,9 @@
       </rPr>
       <t xml:space="preserve">// Root contract ID</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Source ID</t>
   </si>
   <si>
     <r>
@@ -389,18 +392,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A10:AL40"/>
+  <dimension ref="A10:AM40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J14" activeCellId="0" sqref="J14"/>
+      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.97"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="20.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.86"/>
   </cols>
   <sheetData>
     <row r="10" customFormat="false" ht="60" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -413,16 +416,16 @@
       <c r="C10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="G10" s="2" t="s">
         <v>6</v>
       </c>
       <c r="H10" s="1" t="s">
@@ -431,18 +434,20 @@
       <c r="I10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J10" s="3"/>
+      <c r="J10" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="K10" s="3"/>
-      <c r="L10" s="4"/>
+      <c r="L10" s="3"/>
       <c r="M10" s="4"/>
-      <c r="N10" s="5"/>
+      <c r="N10" s="4"/>
       <c r="O10" s="5"/>
       <c r="P10" s="5"/>
-      <c r="Q10" s="6"/>
-      <c r="R10" s="7"/>
+      <c r="Q10" s="5"/>
+      <c r="R10" s="6"/>
       <c r="S10" s="7"/>
-      <c r="T10" s="8"/>
-      <c r="U10" s="9"/>
+      <c r="T10" s="7"/>
+      <c r="U10" s="8"/>
       <c r="V10" s="9"/>
       <c r="W10" s="9"/>
       <c r="X10" s="9"/>
@@ -460,6 +465,7 @@
       <c r="AJ10" s="9"/>
       <c r="AK10" s="9"/>
       <c r="AL10" s="9"/>
+      <c r="AM10" s="9"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="10"/>
@@ -471,6 +477,7 @@
       <c r="G11" s="10"/>
       <c r="H11" s="10"/>
       <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="10"/>
@@ -482,6 +489,7 @@
       <c r="G12" s="10"/>
       <c r="H12" s="10"/>
       <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="10"/>
@@ -493,6 +501,7 @@
       <c r="G13" s="10"/>
       <c r="H13" s="10"/>
       <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="10"/>
@@ -504,6 +513,7 @@
       <c r="G14" s="10"/>
       <c r="H14" s="10"/>
       <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="10"/>
@@ -515,6 +525,7 @@
       <c r="G15" s="10"/>
       <c r="H15" s="10"/>
       <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="10"/>
@@ -526,6 +537,7 @@
       <c r="G16" s="10"/>
       <c r="H16" s="10"/>
       <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="10"/>
@@ -537,6 +549,7 @@
       <c r="G17" s="10"/>
       <c r="H17" s="10"/>
       <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="10"/>
@@ -548,6 +561,7 @@
       <c r="G18" s="10"/>
       <c r="H18" s="10"/>
       <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="10"/>
@@ -559,6 +573,7 @@
       <c r="G19" s="10"/>
       <c r="H19" s="10"/>
       <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="10"/>
@@ -570,6 +585,7 @@
       <c r="G20" s="10"/>
       <c r="H20" s="10"/>
       <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="10"/>
@@ -581,6 +597,7 @@
       <c r="G21" s="10"/>
       <c r="H21" s="10"/>
       <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="10"/>
@@ -592,6 +609,7 @@
       <c r="G22" s="10"/>
       <c r="H22" s="10"/>
       <c r="I22" s="10"/>
+      <c r="J22" s="10"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="10"/>
@@ -603,6 +621,7 @@
       <c r="G23" s="10"/>
       <c r="H23" s="10"/>
       <c r="I23" s="10"/>
+      <c r="J23" s="10"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="10"/>
@@ -614,6 +633,7 @@
       <c r="G24" s="10"/>
       <c r="H24" s="10"/>
       <c r="I24" s="10"/>
+      <c r="J24" s="10"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="10"/>
@@ -625,6 +645,7 @@
       <c r="G25" s="10"/>
       <c r="H25" s="10"/>
       <c r="I25" s="10"/>
+      <c r="J25" s="10"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="10"/>
@@ -636,6 +657,7 @@
       <c r="G26" s="10"/>
       <c r="H26" s="10"/>
       <c r="I26" s="10"/>
+      <c r="J26" s="10"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="10"/>
@@ -647,6 +669,7 @@
       <c r="G27" s="10"/>
       <c r="H27" s="10"/>
       <c r="I27" s="10"/>
+      <c r="J27" s="10"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="10"/>
@@ -658,6 +681,7 @@
       <c r="G28" s="10"/>
       <c r="H28" s="10"/>
       <c r="I28" s="10"/>
+      <c r="J28" s="10"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="10"/>
@@ -669,6 +693,7 @@
       <c r="G29" s="10"/>
       <c r="H29" s="10"/>
       <c r="I29" s="10"/>
+      <c r="J29" s="10"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="10"/>
@@ -680,6 +705,7 @@
       <c r="G30" s="10"/>
       <c r="H30" s="10"/>
       <c r="I30" s="10"/>
+      <c r="J30" s="10"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="10"/>
@@ -691,6 +717,7 @@
       <c r="G31" s="10"/>
       <c r="H31" s="10"/>
       <c r="I31" s="10"/>
+      <c r="J31" s="10"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="10"/>
@@ -702,6 +729,7 @@
       <c r="G32" s="10"/>
       <c r="H32" s="10"/>
       <c r="I32" s="10"/>
+      <c r="J32" s="10"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="10"/>
@@ -713,6 +741,7 @@
       <c r="G33" s="10"/>
       <c r="H33" s="10"/>
       <c r="I33" s="10"/>
+      <c r="J33" s="10"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="10"/>
@@ -724,6 +753,7 @@
       <c r="G34" s="10"/>
       <c r="H34" s="10"/>
       <c r="I34" s="10"/>
+      <c r="J34" s="10"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="10"/>
@@ -735,6 +765,7 @@
       <c r="G35" s="10"/>
       <c r="H35" s="10"/>
       <c r="I35" s="10"/>
+      <c r="J35" s="10"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="10"/>
@@ -746,6 +777,7 @@
       <c r="G36" s="10"/>
       <c r="H36" s="10"/>
       <c r="I36" s="10"/>
+      <c r="J36" s="10"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="10"/>
@@ -757,6 +789,7 @@
       <c r="G37" s="10"/>
       <c r="H37" s="10"/>
       <c r="I37" s="10"/>
+      <c r="J37" s="10"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="10"/>
@@ -768,6 +801,7 @@
       <c r="G38" s="10"/>
       <c r="H38" s="10"/>
       <c r="I38" s="10"/>
+      <c r="J38" s="10"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="10"/>
@@ -779,6 +813,7 @@
       <c r="G39" s="10"/>
       <c r="H39" s="10"/>
       <c r="I39" s="10"/>
+      <c r="J39" s="10"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="10"/>
@@ -790,6 +825,7 @@
       <c r="G40" s="10"/>
       <c r="H40" s="10"/>
       <c r="I40" s="10"/>
+      <c r="J40" s="10"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>